<commit_message>
Clase descripcion.java hecha a falta de algun retoque Carpeta "images" para poner los iconos de cada una de las pantallas
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ene" sheetId="1" r:id="rId1"/>
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="38">
   <si>
     <t>GP</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>Familarizacion con el entorno Git</t>
+  </si>
+  <si>
+    <t>Implementacion de la clase descripcion.java</t>
+  </si>
+  <si>
+    <t>Comienzo de la clase descripcion.java</t>
   </si>
 </sst>
 </file>
@@ -1453,10 +1459,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1479,6 +1481,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1910,7 +1916,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2000,11 +2006,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80609280"/>
-        <c:axId val="80611584"/>
+        <c:axId val="49569152"/>
+        <c:axId val="49579904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80609280"/>
+        <c:axId val="49569152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,13 +2046,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80611584"/>
+        <c:crossAx val="49579904"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80611584"/>
+        <c:axId val="49579904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2097,7 +2103,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80609280"/>
+        <c:crossAx val="49569152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2118,7 +2124,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2131,7 +2137,7 @@
     <xdr:ext cx="10191750" cy="5562600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1" descr="Chart 0"/>
+        <xdr:cNvPr id="2" name="Chart 1" descr="Chart 0"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2495,8 +2501,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="122"/>
+      <c r="AR1" s="141"/>
+      <c r="AS1" s="142"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -5180,8 +5186,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="122"/>
+      <c r="AR1" s="141"/>
+      <c r="AS1" s="142"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -8012,8 +8018,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="121"/>
-      <c r="AR1" s="122"/>
+      <c r="AQ1" s="141"/>
+      <c r="AR1" s="142"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -10797,8 +10803,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="122"/>
+      <c r="AR1" s="141"/>
+      <c r="AS1" s="142"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -13781,7 +13787,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -13797,7 +13803,7 @@
       </c>
       <c r="K6" s="116">
         <f>Abr!G36</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
@@ -14413,8 +14419,8 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="121"/>
-      <c r="AP1" s="122"/>
+      <c r="AO1" s="141"/>
+      <c r="AP1" s="142"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
@@ -14554,55 +14560,55 @@
     </row>
     <row r="3" spans="1:52" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="123">
+      <c r="B3" s="121">
         <v>84</v>
       </c>
-      <c r="C3" s="124">
+      <c r="C3" s="122">
         <v>2</v>
       </c>
-      <c r="D3" s="124">
+      <c r="D3" s="122">
         <v>45</v>
       </c>
-      <c r="E3" s="125">
-        <v>0</v>
-      </c>
-      <c r="F3" s="126" t="s">
+      <c r="E3" s="123">
+        <v>0</v>
+      </c>
+      <c r="F3" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="127">
+      <c r="G3" s="125">
         <f t="shared" ref="G3:G6" si="0">SUM(H3:AI3)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="128"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="128"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="129"/>
-      <c r="S3" s="129"/>
-      <c r="T3" s="129"/>
-      <c r="U3" s="128"/>
-      <c r="V3" s="128"/>
-      <c r="W3" s="130">
+      <c r="H3" s="126"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="127"/>
+      <c r="Q3" s="127"/>
+      <c r="R3" s="127"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="127"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="128">
         <v>1</v>
       </c>
-      <c r="X3" s="129"/>
-      <c r="Y3" s="129"/>
-      <c r="Z3" s="129"/>
-      <c r="AA3" s="129"/>
-      <c r="AB3" s="128"/>
-      <c r="AC3" s="128"/>
-      <c r="AD3" s="129"/>
-      <c r="AE3" s="129"/>
-      <c r="AF3" s="129"/>
-      <c r="AG3" s="129"/>
-      <c r="AH3" s="129"/>
-      <c r="AI3" s="128"/>
+      <c r="X3" s="127"/>
+      <c r="Y3" s="127"/>
+      <c r="Z3" s="127"/>
+      <c r="AA3" s="127"/>
+      <c r="AB3" s="126"/>
+      <c r="AC3" s="126"/>
+      <c r="AD3" s="127"/>
+      <c r="AE3" s="127"/>
+      <c r="AF3" s="127"/>
+      <c r="AG3" s="127"/>
+      <c r="AH3" s="127"/>
+      <c r="AI3" s="126"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
@@ -14623,55 +14629,55 @@
     </row>
     <row r="4" spans="1:52" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="131">
+      <c r="B4" s="129">
         <v>84</v>
       </c>
-      <c r="C4" s="132">
+      <c r="C4" s="130">
         <v>2</v>
       </c>
-      <c r="D4" s="132">
+      <c r="D4" s="130">
         <v>41</v>
       </c>
-      <c r="E4" s="133">
-        <v>0</v>
-      </c>
-      <c r="F4" s="134" t="s">
+      <c r="E4" s="131">
+        <v>0</v>
+      </c>
+      <c r="F4" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="127">
+      <c r="G4" s="125">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H4" s="135"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="136"/>
-      <c r="L4" s="136"/>
-      <c r="M4" s="136"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="136"/>
-      <c r="Q4" s="136"/>
-      <c r="R4" s="136"/>
-      <c r="S4" s="136"/>
-      <c r="T4" s="136"/>
-      <c r="U4" s="135"/>
-      <c r="V4" s="135"/>
-      <c r="W4" s="136"/>
-      <c r="X4" s="136"/>
-      <c r="Y4" s="136"/>
-      <c r="Z4" s="137">
+      <c r="H4" s="133"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="134"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="134"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="134"/>
+      <c r="Q4" s="134"/>
+      <c r="R4" s="134"/>
+      <c r="S4" s="134"/>
+      <c r="T4" s="134"/>
+      <c r="U4" s="133"/>
+      <c r="V4" s="133"/>
+      <c r="W4" s="134"/>
+      <c r="X4" s="134"/>
+      <c r="Y4" s="134"/>
+      <c r="Z4" s="135">
         <v>1</v>
       </c>
-      <c r="AA4" s="136"/>
-      <c r="AB4" s="135"/>
-      <c r="AC4" s="135"/>
-      <c r="AD4" s="136"/>
-      <c r="AE4" s="136"/>
-      <c r="AF4" s="136"/>
-      <c r="AG4" s="136"/>
-      <c r="AH4" s="136"/>
-      <c r="AI4" s="135"/>
+      <c r="AA4" s="134"/>
+      <c r="AB4" s="133"/>
+      <c r="AC4" s="133"/>
+      <c r="AD4" s="134"/>
+      <c r="AE4" s="134"/>
+      <c r="AF4" s="134"/>
+      <c r="AG4" s="134"/>
+      <c r="AH4" s="134"/>
+      <c r="AI4" s="133"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
@@ -14692,55 +14698,55 @@
     </row>
     <row r="5" spans="1:52" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="131">
+      <c r="B5" s="129">
         <v>84</v>
       </c>
-      <c r="C5" s="132">
+      <c r="C5" s="130">
         <v>2</v>
       </c>
-      <c r="D5" s="132">
+      <c r="D5" s="130">
         <v>41</v>
       </c>
-      <c r="E5" s="133">
-        <v>0</v>
-      </c>
-      <c r="F5" s="134" t="s">
+      <c r="E5" s="131">
+        <v>0</v>
+      </c>
+      <c r="F5" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="127">
+      <c r="G5" s="125">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H5" s="135"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="135"/>
-      <c r="O5" s="135"/>
-      <c r="P5" s="136"/>
-      <c r="Q5" s="136"/>
-      <c r="R5" s="136"/>
-      <c r="S5" s="136"/>
-      <c r="T5" s="136"/>
-      <c r="U5" s="135"/>
-      <c r="V5" s="135"/>
-      <c r="W5" s="136"/>
-      <c r="X5" s="136"/>
-      <c r="Y5" s="136"/>
-      <c r="Z5" s="137">
+      <c r="H5" s="133"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="133"/>
+      <c r="O5" s="133"/>
+      <c r="P5" s="134"/>
+      <c r="Q5" s="134"/>
+      <c r="R5" s="134"/>
+      <c r="S5" s="134"/>
+      <c r="T5" s="134"/>
+      <c r="U5" s="133"/>
+      <c r="V5" s="133"/>
+      <c r="W5" s="134"/>
+      <c r="X5" s="134"/>
+      <c r="Y5" s="134"/>
+      <c r="Z5" s="135">
         <v>2</v>
       </c>
-      <c r="AA5" s="136"/>
-      <c r="AB5" s="135"/>
-      <c r="AC5" s="135"/>
-      <c r="AD5" s="136"/>
-      <c r="AE5" s="136"/>
-      <c r="AF5" s="136"/>
-      <c r="AG5" s="136"/>
-      <c r="AH5" s="136"/>
-      <c r="AI5" s="135"/>
+      <c r="AA5" s="134"/>
+      <c r="AB5" s="133"/>
+      <c r="AC5" s="133"/>
+      <c r="AD5" s="134"/>
+      <c r="AE5" s="134"/>
+      <c r="AF5" s="134"/>
+      <c r="AG5" s="134"/>
+      <c r="AH5" s="134"/>
+      <c r="AI5" s="133"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
@@ -14761,55 +14767,55 @@
     </row>
     <row r="6" spans="1:52" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="138">
+      <c r="B6" s="136">
         <v>84</v>
       </c>
-      <c r="C6" s="139">
+      <c r="C6" s="137">
         <v>2</v>
       </c>
-      <c r="D6" s="139">
+      <c r="D6" s="137">
         <v>42</v>
       </c>
-      <c r="E6" s="140">
-        <v>0</v>
-      </c>
-      <c r="F6" s="141" t="s">
+      <c r="E6" s="138">
+        <v>0</v>
+      </c>
+      <c r="F6" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="127">
+      <c r="G6" s="125">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H6" s="135"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="136"/>
-      <c r="Q6" s="136"/>
-      <c r="R6" s="136"/>
-      <c r="S6" s="136"/>
-      <c r="T6" s="136"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="136"/>
-      <c r="X6" s="136"/>
-      <c r="Y6" s="136"/>
-      <c r="Z6" s="136"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="135"/>
-      <c r="AC6" s="135">
+      <c r="H6" s="133"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="133"/>
+      <c r="O6" s="133"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="133"/>
+      <c r="V6" s="133"/>
+      <c r="W6" s="134"/>
+      <c r="X6" s="134"/>
+      <c r="Y6" s="134"/>
+      <c r="Z6" s="134"/>
+      <c r="AA6" s="134"/>
+      <c r="AB6" s="133"/>
+      <c r="AC6" s="133">
         <v>0.5</v>
       </c>
-      <c r="AD6" s="136"/>
-      <c r="AE6" s="136"/>
-      <c r="AF6" s="136"/>
-      <c r="AG6" s="136"/>
-      <c r="AH6" s="136"/>
-      <c r="AI6" s="135"/>
+      <c r="AD6" s="134"/>
+      <c r="AE6" s="134"/>
+      <c r="AF6" s="134"/>
+      <c r="AG6" s="134"/>
+      <c r="AH6" s="134"/>
+      <c r="AI6" s="133"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
@@ -14836,7 +14842,7 @@
       <c r="E7" s="24"/>
       <c r="F7" s="25"/>
       <c r="G7" s="15">
-        <f t="shared" ref="G6:G36" si="1">SUM(H7:AI7)</f>
+        <f t="shared" ref="G7:G36" si="1">SUM(H7:AI7)</f>
         <v>0</v>
       </c>
       <c r="H7" s="19"/>
@@ -17038,7 +17044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -17098,8 +17104,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="122"/>
+      <c r="AR1" s="141"/>
+      <c r="AS1" s="142"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -17248,43 +17254,43 @@
     </row>
     <row r="3" spans="1:55" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="138">
+      <c r="B3" s="136">
         <v>84</v>
       </c>
-      <c r="C3" s="139">
+      <c r="C3" s="137">
         <v>2</v>
       </c>
-      <c r="D3" s="139">
+      <c r="D3" s="137">
         <v>42</v>
       </c>
-      <c r="E3" s="140">
-        <v>0</v>
-      </c>
-      <c r="F3" s="141" t="s">
+      <c r="E3" s="138">
+        <v>0</v>
+      </c>
+      <c r="F3" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="127">
+      <c r="G3" s="125">
         <f t="shared" ref="G3:G4" si="0">SUM(H3:AL3)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="128"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="142"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="128"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="142"/>
-      <c r="Q3" s="142"/>
-      <c r="R3" s="142"/>
-      <c r="S3" s="142">
+      <c r="H3" s="126"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="140"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140">
         <v>1</v>
       </c>
-      <c r="T3" s="142"/>
-      <c r="U3" s="128"/>
-      <c r="V3" s="128"/>
-      <c r="W3" s="142"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="140"/>
       <c r="X3" s="48"/>
       <c r="Y3" s="48"/>
       <c r="Z3" s="48"/>
@@ -17320,43 +17326,43 @@
     </row>
     <row r="4" spans="1:55" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="138">
+      <c r="B4" s="136">
         <v>84</v>
       </c>
-      <c r="C4" s="139">
+      <c r="C4" s="137">
         <v>2</v>
       </c>
-      <c r="D4" s="139">
+      <c r="D4" s="137">
         <v>42</v>
       </c>
-      <c r="E4" s="140">
-        <v>0</v>
-      </c>
-      <c r="F4" s="141" t="s">
+      <c r="E4" s="138">
+        <v>0</v>
+      </c>
+      <c r="F4" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="127">
+      <c r="G4" s="125">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="H4" s="135"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="135"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="139"/>
-      <c r="Q4" s="139"/>
-      <c r="R4" s="139"/>
-      <c r="S4" s="139">
+      <c r="H4" s="133"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="137"/>
+      <c r="Q4" s="137"/>
+      <c r="R4" s="137"/>
+      <c r="S4" s="137">
         <v>2.5</v>
       </c>
-      <c r="T4" s="139"/>
-      <c r="U4" s="135"/>
-      <c r="V4" s="135"/>
-      <c r="W4" s="139"/>
+      <c r="T4" s="137"/>
+      <c r="U4" s="133"/>
+      <c r="V4" s="133"/>
+      <c r="W4" s="137"/>
       <c r="X4" s="23"/>
       <c r="Y4" s="23"/>
       <c r="Z4" s="23"/>
@@ -17408,7 +17414,7 @@
         <v>35</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" ref="G3:G36" si="1">SUM(H5:AL5)</f>
+        <f t="shared" ref="G5:G36" si="1">SUM(H5:AL5)</f>
         <v>0.5</v>
       </c>
       <c r="H5" s="19"/>
@@ -19852,7 +19858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BB43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -19909,8 +19917,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="121"/>
-      <c r="AR1" s="122"/>
+      <c r="AQ1" s="141"/>
+      <c r="AR1" s="142"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -20056,14 +20064,24 @@
     </row>
     <row r="3" spans="1:54" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="54"/>
+      <c r="B3" s="17">
+        <v>84</v>
+      </c>
+      <c r="C3" s="48">
+        <v>2</v>
+      </c>
+      <c r="D3" s="48">
+        <v>52</v>
+      </c>
+      <c r="E3" s="53">
+        <v>0</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="15">
         <f t="shared" ref="G3:G36" si="0">SUM(H3:AK3)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -20076,7 +20094,9 @@
       <c r="P3" s="48"/>
       <c r="Q3" s="48"/>
       <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
+      <c r="S3" s="16">
+        <v>0.5</v>
+      </c>
       <c r="T3" s="48"/>
       <c r="U3" s="48"/>
       <c r="V3" s="48"/>
@@ -20115,14 +20135,24 @@
     </row>
     <row r="4" spans="1:54" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="B4" s="17">
+        <v>84</v>
+      </c>
+      <c r="C4" s="48">
+        <v>2</v>
+      </c>
+      <c r="D4" s="48">
+        <v>52</v>
+      </c>
+      <c r="E4" s="53">
+        <v>0</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>36</v>
+      </c>
       <c r="G4" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
@@ -20137,7 +20167,9 @@
       <c r="R4" s="19"/>
       <c r="S4" s="19"/>
       <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
+      <c r="U4" s="23">
+        <v>1</v>
+      </c>
       <c r="V4" s="23"/>
       <c r="W4" s="23"/>
       <c r="X4" s="23"/>
@@ -22012,7 +22044,7 @@
       </c>
       <c r="G36" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H36" s="37">
         <f t="shared" ref="H36:AK36" si="1">SUM(H3:H35)</f>
@@ -22060,7 +22092,7 @@
       </c>
       <c r="S36" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T36" s="72">
         <f t="shared" si="1"/>
@@ -22068,7 +22100,7 @@
       </c>
       <c r="U36" s="72">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V36" s="72">
         <f t="shared" si="1"/>
@@ -22638,8 +22670,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="122"/>
+      <c r="AR1" s="141"/>
+      <c r="AS1" s="142"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -25413,8 +25445,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="121"/>
-      <c r="AR1" s="122"/>
+      <c r="AQ1" s="141"/>
+      <c r="AR1" s="142"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -28143,8 +28175,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="122"/>
+      <c r="AR1" s="141"/>
+      <c r="AS1" s="142"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -30919,8 +30951,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="122"/>
+      <c r="AR1" s="141"/>
+      <c r="AS1" s="142"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -33694,8 +33726,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="121"/>
-      <c r="AR1" s="122"/>
+      <c r="AQ1" s="141"/>
+      <c r="AR1" s="142"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>

</xml_diff>

<commit_message>
Modificacion clase Descripcion y clase View ( comentado de los metodos) Hoja de esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="41">
   <si>
     <t>GP</t>
   </si>
@@ -430,6 +430,15 @@
   </si>
   <si>
     <t>Comienzo de la clase descripcion.java</t>
+  </si>
+  <si>
+    <t>Cambios en la clase Descripcion, y View</t>
+  </si>
+  <si>
+    <t>Practica 3. Planificación de auditoria.</t>
+  </si>
+  <si>
+    <t>Reunion con el profesor sobre la calidad</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1481,15 +1490,300 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1916,7 +2210,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2006,11 +2300,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="49569152"/>
-        <c:axId val="49579904"/>
+        <c:axId val="74804608"/>
+        <c:axId val="74815360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49569152"/>
+        <c:axId val="74804608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2046,13 +2340,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49579904"/>
+        <c:crossAx val="74815360"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49579904"/>
+        <c:axId val="74815360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2397,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49569152"/>
+        <c:crossAx val="74804608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2124,7 +2418,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2501,8 +2795,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="143"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -5110,12 +5404,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5186,8 +5480,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="143"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -7943,12 +8237,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8018,8 +8312,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="141"/>
-      <c r="AR1" s="142"/>
+      <c r="AQ1" s="142"/>
+      <c r="AR1" s="143"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -10727,12 +11021,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10803,8 +11097,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="143"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -13560,12 +13854,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13787,7 +14081,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -13803,7 +14097,7 @@
       </c>
       <c r="K6" s="116">
         <f>Abr!G36</f>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
@@ -14344,12 +14638,12 @@
     <row r="39" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14419,8 +14713,8 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="141"/>
-      <c r="AP1" s="142"/>
+      <c r="AO1" s="142"/>
+      <c r="AP1" s="143"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
@@ -17026,12 +17320,12 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17045,7 +17339,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -17104,8 +17398,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="143"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -19840,12 +20134,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19859,7 +20153,7 @@
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -19917,8 +20211,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="141"/>
-      <c r="AR1" s="142"/>
+      <c r="AQ1" s="142"/>
+      <c r="AR1" s="143"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -20062,66 +20356,65 @@
       <c r="BA2" s="2"/>
       <c r="BB2" s="2"/>
     </row>
-    <row r="3" spans="1:54" ht="13.5" customHeight="1">
+    <row r="3" spans="1:54" s="147" customFormat="1" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="17">
+      <c r="B3" s="144">
         <v>84</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="145">
         <v>2</v>
       </c>
-      <c r="D3" s="48">
-        <v>52</v>
-      </c>
-      <c r="E3" s="53">
-        <v>0</v>
-      </c>
-      <c r="F3" s="54" t="s">
-        <v>37</v>
+      <c r="D3" s="145">
+        <v>44</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0</v>
+      </c>
+      <c r="F3" s="146" t="s">
+        <v>40</v>
       </c>
       <c r="G3" s="15">
-        <f t="shared" ref="G3:G36" si="0">SUM(H3:AK3)</f>
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="48"/>
-      <c r="AC3" s="48"/>
-      <c r="AD3" s="16"/>
-      <c r="AE3" s="16"/>
-      <c r="AF3" s="16"/>
-      <c r="AG3" s="16"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
+        <v>1</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="145">
+        <v>1</v>
+      </c>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="17"/>
-      <c r="AR3" s="18"/>
+      <c r="AQ3" s="21"/>
+      <c r="AR3" s="22"/>
       <c r="AS3" s="1"/>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
@@ -20133,7 +20426,7 @@
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
     </row>
-    <row r="4" spans="1:54" ht="13.5" customHeight="1">
+    <row r="4" spans="1:54" s="141" customFormat="1" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="17">
         <v>84</v>
@@ -20142,57 +20435,57 @@
         <v>2</v>
       </c>
       <c r="D4" s="48">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E4" s="53">
         <v>0</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23">
-        <v>1</v>
-      </c>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="23"/>
+        <f t="shared" ref="G4:G7" si="0">SUM(H4:AK4)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="48"/>
+      <c r="AK4" s="48"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="21"/>
-      <c r="AR4" s="22"/>
+      <c r="AQ4" s="17"/>
+      <c r="AR4" s="18"/>
       <c r="AS4" s="1"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
@@ -20204,16 +20497,26 @@
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
     </row>
-    <row r="5" spans="1:54" ht="13.5" customHeight="1">
+    <row r="5" spans="1:54" s="141" customFormat="1" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="17">
+        <v>84</v>
+      </c>
+      <c r="C5" s="48">
+        <v>2</v>
+      </c>
+      <c r="D5" s="48">
+        <v>54</v>
+      </c>
+      <c r="E5" s="53">
+        <v>0</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>36</v>
+      </c>
       <c r="G5" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -20228,7 +20531,9 @@
       <c r="R5" s="19"/>
       <c r="S5" s="19"/>
       <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
+      <c r="U5" s="23">
+        <v>1</v>
+      </c>
       <c r="V5" s="23"/>
       <c r="W5" s="23"/>
       <c r="X5" s="23"/>
@@ -20263,16 +20568,26 @@
       <c r="BA5" s="1"/>
       <c r="BB5" s="1"/>
     </row>
-    <row r="6" spans="1:54" ht="13.5" customHeight="1">
+    <row r="6" spans="1:54" s="141" customFormat="1" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="144">
+        <v>84</v>
+      </c>
+      <c r="C6" s="145">
+        <v>2</v>
+      </c>
+      <c r="D6" s="145">
+        <v>44</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="146" t="s">
+        <v>39</v>
+      </c>
       <c r="G6" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(H6:AK6)</f>
+        <v>2</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -20288,7 +20603,9 @@
       <c r="S6" s="19"/>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
+      <c r="V6" s="145">
+        <v>2</v>
+      </c>
       <c r="W6" s="23"/>
       <c r="X6" s="23"/>
       <c r="Y6" s="19"/>
@@ -20322,16 +20639,26 @@
       <c r="BA6" s="1"/>
       <c r="BB6" s="1"/>
     </row>
-    <row r="7" spans="1:54" ht="13.5" customHeight="1">
+    <row r="7" spans="1:54" s="141" customFormat="1" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="21">
+        <v>84</v>
+      </c>
+      <c r="C7" s="23">
+        <v>2</v>
+      </c>
+      <c r="D7" s="23">
+        <v>54</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>38</v>
+      </c>
       <c r="G7" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="G7" si="1">SUM(H7:AK7)</f>
+        <v>1</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -20350,7 +20677,9 @@
       <c r="V7" s="23"/>
       <c r="W7" s="23"/>
       <c r="X7" s="23"/>
-      <c r="Y7" s="19"/>
+      <c r="Y7" s="19">
+        <v>1</v>
+      </c>
       <c r="Z7" s="19"/>
       <c r="AA7" s="23"/>
       <c r="AB7" s="23"/>
@@ -20381,17 +20710,14 @@
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
     </row>
-    <row r="8" spans="1:54" ht="13.5" customHeight="1">
+    <row r="8" spans="1:54" s="147" customFormat="1" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="144"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F8" s="146"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -20401,7 +20727,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
+      <c r="Q8" s="145"/>
       <c r="R8" s="19"/>
       <c r="S8" s="19"/>
       <c r="T8" s="23"/>
@@ -20448,7 +20774,7 @@
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
       <c r="G9" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="XFD1048576:A1" si="2">SUM(H9:AK9)</f>
         <v>0</v>
       </c>
       <c r="H9" s="19"/>
@@ -20507,7 +20833,7 @@
       <c r="E10" s="24"/>
       <c r="F10" s="25"/>
       <c r="G10" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10" s="19"/>
@@ -20566,7 +20892,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="25"/>
       <c r="G11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H11" s="19"/>
@@ -20625,7 +20951,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="25"/>
       <c r="G12" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H12" s="19"/>
@@ -20684,7 +21010,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="25"/>
       <c r="G13" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13" s="19"/>
@@ -20743,7 +21069,7 @@
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H14" s="19"/>
@@ -20802,7 +21128,7 @@
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H15" s="19"/>
@@ -20861,7 +21187,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="25"/>
       <c r="G16" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H16" s="19"/>
@@ -20920,7 +21246,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="25"/>
       <c r="G17" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H17" s="19"/>
@@ -20979,7 +21305,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
       <c r="G18" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H18" s="19"/>
@@ -21038,7 +21364,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
       <c r="G19" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H19" s="19"/>
@@ -21097,7 +21423,7 @@
       <c r="E20" s="24"/>
       <c r="F20" s="25"/>
       <c r="G20" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H20" s="19"/>
@@ -21156,7 +21482,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="25"/>
       <c r="G21" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H21" s="19"/>
@@ -21215,7 +21541,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="25"/>
       <c r="G22" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H22" s="19"/>
@@ -21274,7 +21600,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="25"/>
       <c r="G23" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H23" s="19"/>
@@ -21333,7 +21659,7 @@
       <c r="E24" s="24"/>
       <c r="F24" s="25"/>
       <c r="G24" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H24" s="19"/>
@@ -21392,7 +21718,7 @@
       <c r="E25" s="24"/>
       <c r="F25" s="25"/>
       <c r="G25" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25" s="19"/>
@@ -21451,7 +21777,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
       <c r="G26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H26" s="19"/>
@@ -21510,7 +21836,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="25"/>
       <c r="G27" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H27" s="19"/>
@@ -21569,7 +21895,7 @@
       <c r="E28" s="24"/>
       <c r="F28" s="25"/>
       <c r="G28" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H28" s="19"/>
@@ -21628,7 +21954,7 @@
       <c r="E29" s="24"/>
       <c r="F29" s="25"/>
       <c r="G29" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H29" s="19"/>
@@ -21687,7 +22013,7 @@
       <c r="E30" s="24"/>
       <c r="F30" s="25"/>
       <c r="G30" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H30" s="19"/>
@@ -21746,7 +22072,7 @@
       <c r="E31" s="24"/>
       <c r="F31" s="25"/>
       <c r="G31" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H31" s="19"/>
@@ -21805,7 +22131,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="25"/>
       <c r="G32" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H32" s="19"/>
@@ -21864,7 +22190,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
       <c r="G33" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H33" s="19"/>
@@ -21923,7 +22249,7 @@
       <c r="E34" s="24"/>
       <c r="F34" s="25"/>
       <c r="G34" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H34" s="19"/>
@@ -21982,7 +22308,7 @@
       <c r="E35" s="28"/>
       <c r="F35" s="29"/>
       <c r="G35" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H35" s="31"/>
@@ -22043,127 +22369,127 @@
         <v>8</v>
       </c>
       <c r="G36" s="36">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <f t="shared" si="2"/>
+        <v>4.5</v>
       </c>
       <c r="H36" s="37">
-        <f t="shared" ref="H36:AK36" si="1">SUM(H3:H35)</f>
+        <f t="shared" ref="XFD1048576:A1" si="3">SUM(H3:H35)</f>
         <v>0</v>
       </c>
       <c r="I36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="T36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="V36" s="72">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="W36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y36" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Z36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK36" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AL36" s="1"/>
@@ -22594,12 +22920,62 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22670,8 +23046,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="143"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -25370,12 +25746,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25445,8 +25821,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="141"/>
-      <c r="AR1" s="142"/>
+      <c r="AQ1" s="142"/>
+      <c r="AR1" s="143"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -28098,12 +28474,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28175,8 +28551,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="143"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -30875,12 +31251,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30951,8 +31327,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="143"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -33651,12 +34027,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33726,8 +34102,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="141"/>
-      <c r="AR1" s="142"/>
+      <c r="AQ1" s="142"/>
+      <c r="AR1" s="143"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -36379,12 +36755,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Hoja de esfuerzos, modificacion Lecciones Aprendidas.docx, Lecciones Aprendidas.pdf
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
@@ -36,6 +36,7 @@
     <definedName name="Print_Area" localSheetId="8">Sep!$A$1:$AR$37</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -316,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="43">
   <si>
     <t>GP</t>
   </si>
@@ -439,6 +440,12 @@
   </si>
   <si>
     <t>Reunion con el profesor sobre la calidad</t>
+  </si>
+  <si>
+    <t>Reunción de planificación</t>
+  </si>
+  <si>
+    <t>Fichero de lecciones aprendidas</t>
   </si>
 </sst>
 </file>
@@ -1308,7 +1315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1491,103 +1498,20 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2210,7 +2134,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2300,11 +2224,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74804608"/>
-        <c:axId val="74815360"/>
+        <c:axId val="50175360"/>
+        <c:axId val="50198400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74804608"/>
+        <c:axId val="50175360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2340,13 +2264,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74815360"/>
+        <c:crossAx val="50198400"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74815360"/>
+        <c:axId val="50198400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2397,7 +2321,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74804608"/>
+        <c:crossAx val="50175360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2418,7 +2342,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2795,8 +2719,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="143"/>
+      <c r="AR1" s="146"/>
+      <c r="AS1" s="147"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -5404,12 +5328,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5480,8 +5404,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="143"/>
+      <c r="AR1" s="146"/>
+      <c r="AS1" s="147"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -8237,12 +8161,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8312,8 +8236,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="142"/>
-      <c r="AR1" s="143"/>
+      <c r="AQ1" s="146"/>
+      <c r="AR1" s="147"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -11021,12 +10945,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11097,8 +11021,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="143"/>
+      <c r="AR1" s="146"/>
+      <c r="AS1" s="147"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -13854,12 +13778,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14081,7 +14005,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -14097,7 +14021,7 @@
       </c>
       <c r="K6" s="116">
         <f>Abr!G36</f>
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
@@ -14638,12 +14562,12 @@
     <row r="39" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14713,8 +14637,8 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="142"/>
-      <c r="AP1" s="143"/>
+      <c r="AO1" s="146"/>
+      <c r="AP1" s="147"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
@@ -17320,12 +17244,12 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17398,8 +17322,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="143"/>
+      <c r="AR1" s="146"/>
+      <c r="AS1" s="147"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -20134,12 +20058,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20153,7 +20077,7 @@
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -20211,8 +20135,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="142"/>
-      <c r="AR1" s="143"/>
+      <c r="AQ1" s="146"/>
+      <c r="AR1" s="147"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -20356,21 +20280,21 @@
       <c r="BA2" s="2"/>
       <c r="BB2" s="2"/>
     </row>
-    <row r="3" spans="1:54" s="147" customFormat="1" ht="13.5" customHeight="1">
+    <row r="3" spans="1:54" s="145" customFormat="1" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="144">
+      <c r="B3" s="142">
         <v>84</v>
       </c>
-      <c r="C3" s="145">
+      <c r="C3" s="143">
         <v>2</v>
       </c>
-      <c r="D3" s="145">
+      <c r="D3" s="143">
         <v>44</v>
       </c>
       <c r="E3" s="24">
         <v>0</v>
       </c>
-      <c r="F3" s="146" t="s">
+      <c r="F3" s="144" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="15">
@@ -20385,7 +20309,7 @@
       <c r="N3" s="23"/>
       <c r="O3" s="23"/>
       <c r="P3" s="23"/>
-      <c r="Q3" s="145">
+      <c r="Q3" s="143">
         <v>1</v>
       </c>
       <c r="R3" s="19"/>
@@ -20444,7 +20368,7 @@
         <v>37</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" ref="G4:G7" si="0">SUM(H4:AK4)</f>
+        <f t="shared" ref="G4:G5" si="0">SUM(H4:AK4)</f>
         <v>0.5</v>
       </c>
       <c r="H4" s="16"/>
@@ -20570,19 +20494,19 @@
     </row>
     <row r="6" spans="1:54" s="141" customFormat="1" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="144">
+      <c r="B6" s="142">
         <v>84</v>
       </c>
-      <c r="C6" s="145">
+      <c r="C6" s="143">
         <v>2</v>
       </c>
-      <c r="D6" s="145">
+      <c r="D6" s="143">
         <v>44</v>
       </c>
       <c r="E6" s="24">
         <v>0</v>
       </c>
-      <c r="F6" s="146" t="s">
+      <c r="F6" s="144" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="15">
@@ -20603,7 +20527,7 @@
       <c r="S6" s="19"/>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
-      <c r="V6" s="145">
+      <c r="V6" s="143">
         <v>2</v>
       </c>
       <c r="W6" s="23"/>
@@ -20710,14 +20634,27 @@
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
     </row>
-    <row r="8" spans="1:54" s="147" customFormat="1" ht="13.5" customHeight="1">
+    <row r="8" spans="1:54" s="145" customFormat="1" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="144"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="15"/>
+      <c r="B8" s="142">
+        <v>84</v>
+      </c>
+      <c r="C8" s="143">
+        <v>2</v>
+      </c>
+      <c r="D8" s="143">
+        <v>53</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="144" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" ref="G8" si="2">SUM(H8:AK8)</f>
+        <v>0.75</v>
+      </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -20727,7 +20664,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
-      <c r="Q8" s="145"/>
+      <c r="Q8" s="23"/>
       <c r="R8" s="19"/>
       <c r="S8" s="19"/>
       <c r="T8" s="23"/>
@@ -20736,7 +20673,9 @@
       <c r="W8" s="23"/>
       <c r="X8" s="23"/>
       <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
+      <c r="Z8" s="148">
+        <v>0.75</v>
+      </c>
       <c r="AA8" s="23"/>
       <c r="AB8" s="23"/>
       <c r="AC8" s="23"/>
@@ -20768,14 +20707,24 @@
     </row>
     <row r="9" spans="1:54" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="21">
+        <v>84</v>
+      </c>
+      <c r="C9" s="23">
+        <v>2</v>
+      </c>
+      <c r="D9" s="23">
+        <v>45</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="G9" s="15">
-        <f t="shared" ref="XFD1048576:A1" si="2">SUM(H9:AK9)</f>
-        <v>0</v>
+        <f t="shared" ref="G9:G36" si="3">SUM(H9:AK9)</f>
+        <v>0.25</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
@@ -20795,7 +20744,9 @@
       <c r="W9" s="23"/>
       <c r="X9" s="23"/>
       <c r="Y9" s="19"/>
-      <c r="Z9" s="19"/>
+      <c r="Z9" s="19">
+        <v>0.25</v>
+      </c>
       <c r="AA9" s="23"/>
       <c r="AB9" s="23"/>
       <c r="AC9" s="23"/>
@@ -20833,7 +20784,7 @@
       <c r="E10" s="24"/>
       <c r="F10" s="25"/>
       <c r="G10" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H10" s="19"/>
@@ -20892,7 +20843,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="25"/>
       <c r="G11" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H11" s="19"/>
@@ -20951,7 +20902,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="25"/>
       <c r="G12" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H12" s="19"/>
@@ -21010,7 +20961,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="25"/>
       <c r="G13" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13" s="19"/>
@@ -21069,7 +21020,7 @@
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H14" s="19"/>
@@ -21128,7 +21079,7 @@
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H15" s="19"/>
@@ -21187,7 +21138,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="25"/>
       <c r="G16" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H16" s="19"/>
@@ -21246,7 +21197,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="25"/>
       <c r="G17" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H17" s="19"/>
@@ -21305,7 +21256,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
       <c r="G18" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H18" s="19"/>
@@ -21364,7 +21315,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
       <c r="G19" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H19" s="19"/>
@@ -21423,7 +21374,7 @@
       <c r="E20" s="24"/>
       <c r="F20" s="25"/>
       <c r="G20" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H20" s="19"/>
@@ -21482,7 +21433,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="25"/>
       <c r="G21" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H21" s="19"/>
@@ -21541,7 +21492,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="25"/>
       <c r="G22" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H22" s="19"/>
@@ -21600,7 +21551,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="25"/>
       <c r="G23" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H23" s="19"/>
@@ -21659,7 +21610,7 @@
       <c r="E24" s="24"/>
       <c r="F24" s="25"/>
       <c r="G24" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H24" s="19"/>
@@ -21718,7 +21669,7 @@
       <c r="E25" s="24"/>
       <c r="F25" s="25"/>
       <c r="G25" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H25" s="19"/>
@@ -21777,7 +21728,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
       <c r="G26" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26" s="19"/>
@@ -21836,7 +21787,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="25"/>
       <c r="G27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H27" s="19"/>
@@ -21895,7 +21846,7 @@
       <c r="E28" s="24"/>
       <c r="F28" s="25"/>
       <c r="G28" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H28" s="19"/>
@@ -21954,7 +21905,7 @@
       <c r="E29" s="24"/>
       <c r="F29" s="25"/>
       <c r="G29" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H29" s="19"/>
@@ -22013,7 +21964,7 @@
       <c r="E30" s="24"/>
       <c r="F30" s="25"/>
       <c r="G30" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H30" s="19"/>
@@ -22072,7 +22023,7 @@
       <c r="E31" s="24"/>
       <c r="F31" s="25"/>
       <c r="G31" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H31" s="19"/>
@@ -22131,7 +22082,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="25"/>
       <c r="G32" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H32" s="19"/>
@@ -22190,7 +22141,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
       <c r="G33" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H33" s="19"/>
@@ -22249,7 +22200,7 @@
       <c r="E34" s="24"/>
       <c r="F34" s="25"/>
       <c r="G34" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H34" s="19"/>
@@ -22308,7 +22259,7 @@
       <c r="E35" s="28"/>
       <c r="F35" s="29"/>
       <c r="G35" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H35" s="31"/>
@@ -22369,127 +22320,127 @@
         <v>8</v>
       </c>
       <c r="G36" s="36">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
+        <f t="shared" si="3"/>
+        <v>6.5</v>
       </c>
       <c r="H36" s="37">
-        <f t="shared" ref="XFD1048576:A1" si="3">SUM(H3:H35)</f>
+        <f t="shared" ref="H36:AK36" si="4">SUM(H3:H35)</f>
         <v>0</v>
       </c>
       <c r="I36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q36" s="72">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="R36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="T36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="W36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Y36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Z36" s="37">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="AA36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AB36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG36" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AK36" s="72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AL36" s="1"/>
@@ -22920,61 +22871,71 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="11" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
+  <conditionalFormatting sqref="G8">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -23046,8 +23007,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="143"/>
+      <c r="AR1" s="146"/>
+      <c r="AS1" s="147"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -25746,12 +25707,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25821,8 +25782,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="142"/>
-      <c r="AR1" s="143"/>
+      <c r="AQ1" s="146"/>
+      <c r="AR1" s="147"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -28474,12 +28435,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28551,8 +28512,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="143"/>
+      <c r="AR1" s="146"/>
+      <c r="AS1" s="147"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -31251,12 +31212,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31327,8 +31288,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="143"/>
+      <c r="AR1" s="146"/>
+      <c r="AS1" s="147"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -34027,12 +33988,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34102,8 +34063,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="142"/>
-      <c r="AR1" s="143"/>
+      <c r="AQ1" s="146"/>
+      <c r="AR1" s="147"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
@@ -36755,12 +36716,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Corregidos vista de la app Administrador y Cliente Hoja de esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="48">
   <si>
     <t>GP</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>Funcionalidad de modificar un modelo para el administrador(Problemas version JAVA)</t>
+  </si>
+  <si>
+    <t>Reuncion para preparar la presentacion</t>
+  </si>
+  <si>
+    <t>Corregido vista de la aplicación Administrador y Cliente</t>
   </si>
 </sst>
 </file>
@@ -1564,12 +1570,40 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="46">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFCCFFFF"/>
           <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
         </patternFill>
       </fill>
       <border>
@@ -2251,7 +2285,7 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2338,11 +2372,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74155520"/>
-        <c:axId val="74157440"/>
+        <c:axId val="72731264"/>
+        <c:axId val="72737536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74155520"/>
+        <c:axId val="72731264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2378,13 +2412,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74157440"/>
+        <c:crossAx val="72737536"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74157440"/>
+        <c:axId val="72737536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2435,7 +2469,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74155520"/>
+        <c:crossAx val="72731264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2457,7 +2491,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6019,12 +6053,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8853,12 +8887,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11638,12 +11672,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14472,12 +14506,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14700,7 +14734,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>18</v>
+        <v>19.25</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -14720,7 +14754,7 @@
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
-        <v>3</v>
+        <v>4.25</v>
       </c>
       <c r="M6" s="116">
         <f>Jun!G36</f>
@@ -15257,12 +15291,12 @@
     <row r="39" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17939,12 +17973,12 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20754,12 +20788,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23568,72 +23602,72 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="37" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="36" priority="14" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="14" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="31" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23648,7 +23682,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24017,7 +24051,7 @@
         <v>45</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" ref="G5" si="2">SUM(H5:AL5)</f>
+        <f t="shared" ref="G5:G6" si="2">SUM(H5:AL5)</f>
         <v>1</v>
       </c>
       <c r="H5" s="19"/>
@@ -24071,16 +24105,26 @@
       <c r="BB5" s="1"/>
       <c r="BC5" s="1"/>
     </row>
-    <row r="6" spans="1:55" ht="13.5" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+    <row r="6" spans="1:55" s="151" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A6" s="148"/>
+      <c r="B6" s="21">
+        <v>84</v>
+      </c>
+      <c r="C6" s="23">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>58</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="G6" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -24095,7 +24139,9 @@
       <c r="R6" s="23"/>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
+      <c r="U6" s="23">
+        <v>1</v>
+      </c>
       <c r="V6" s="23"/>
       <c r="W6" s="19"/>
       <c r="X6" s="19"/>
@@ -24113,34 +24159,44 @@
       <c r="AJ6" s="23"/>
       <c r="AK6" s="19"/>
       <c r="AL6" s="19"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
+      <c r="AM6" s="148"/>
+      <c r="AN6" s="148"/>
+      <c r="AO6" s="148"/>
+      <c r="AP6" s="148"/>
+      <c r="AQ6" s="148"/>
       <c r="AR6" s="21"/>
       <c r="AS6" s="22"/>
-      <c r="AT6" s="1"/>
-      <c r="AU6" s="1"/>
-      <c r="AV6" s="1"/>
-      <c r="AW6" s="1"/>
-      <c r="AX6" s="1"/>
-      <c r="AY6" s="1"/>
-      <c r="AZ6" s="1"/>
-      <c r="BA6" s="1"/>
-      <c r="BB6" s="1"/>
-      <c r="BC6" s="1"/>
+      <c r="AT6" s="148"/>
+      <c r="AU6" s="148"/>
+      <c r="AV6" s="148"/>
+      <c r="AW6" s="148"/>
+      <c r="AX6" s="148"/>
+      <c r="AY6" s="148"/>
+      <c r="AZ6" s="148"/>
+      <c r="BA6" s="148"/>
+      <c r="BB6" s="148"/>
+      <c r="BC6" s="148"/>
     </row>
     <row r="7" spans="1:55" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="21">
+        <v>84</v>
+      </c>
+      <c r="C7" s="23">
+        <v>2</v>
+      </c>
+      <c r="D7" s="23">
+        <v>54</v>
+      </c>
+      <c r="E7" s="24">
+        <v>5</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>47</v>
+      </c>
       <c r="G7" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -24157,7 +24213,9 @@
       <c r="T7" s="23"/>
       <c r="U7" s="23"/>
       <c r="V7" s="23"/>
-      <c r="W7" s="19"/>
+      <c r="W7" s="19">
+        <v>0.25</v>
+      </c>
       <c r="X7" s="19"/>
       <c r="Y7" s="23"/>
       <c r="Z7" s="23"/>
@@ -25882,7 +25940,7 @@
       </c>
       <c r="G36" s="36">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4.25</v>
       </c>
       <c r="H36" s="37">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -25938,7 +25996,7 @@
       </c>
       <c r="U36" s="72">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V36" s="72">
         <f t="shared" si="3"/>
@@ -25946,7 +26004,7 @@
       </c>
       <c r="W36" s="37">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="X36" s="37">
         <f t="shared" si="3"/>
@@ -26443,12 +26501,22 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26462,13 +26530,13 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29192,12 +29260,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31970,12 +32038,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34747,12 +34815,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37476,12 +37544,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Hoja de esfuerzos y la de equipo
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="50">
   <si>
     <t>GP</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>Reunion para preparar la presentacion</t>
+  </si>
+  <si>
+    <t>Reunion para preparar la presentacion tecnica y reparto de tareas</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1576,35 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2218,11 +2249,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="es-ES"/>
               <a:t>Gráfica Esfuerzos totales/Formación</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2260,7 +2293,7 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.75</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2347,11 +2380,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="47358720"/>
-        <c:axId val="47361024"/>
+        <c:axId val="76131712"/>
+        <c:axId val="76171136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47358720"/>
+        <c:axId val="76131712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2370,11 +2403,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="es-ES"/>
                   <a:t>Mes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -2387,13 +2422,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47361024"/>
+        <c:crossAx val="76171136"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47361024"/>
+        <c:axId val="76171136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2421,11 +2456,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="es-ES"/>
                   <a:t>Horas</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2444,7 +2481,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47358720"/>
+        <c:crossAx val="76131712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2456,6 +2493,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -2466,7 +2504,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6028,12 +6066,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8862,12 +8900,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11647,12 +11685,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14481,12 +14519,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14709,7 +14747,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>19.75</v>
+        <v>20.75</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -14729,7 +14767,7 @@
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
-        <v>4.75</v>
+        <v>5.75</v>
       </c>
       <c r="M6" s="116">
         <f>Jun!G36</f>
@@ -15266,12 +15304,12 @@
     <row r="39" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17948,12 +17986,12 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20763,12 +20801,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23577,72 +23615,72 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="37" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="36" priority="14" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="14" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="31" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23657,7 +23695,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24296,16 +24334,26 @@
       <c r="BB8" s="1"/>
       <c r="BC8" s="1"/>
     </row>
-    <row r="9" spans="1:55" ht="13.5" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+    <row r="9" spans="1:55" s="151" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A9" s="148"/>
+      <c r="B9" s="21">
+        <v>84</v>
+      </c>
+      <c r="C9" s="23">
+        <v>2</v>
+      </c>
+      <c r="D9" s="23">
+        <v>58</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>49</v>
+      </c>
       <c r="G9" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
@@ -24324,7 +24372,9 @@
       <c r="V9" s="23"/>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
-      <c r="Y9" s="23"/>
+      <c r="Y9" s="23">
+        <v>1</v>
+      </c>
       <c r="Z9" s="23"/>
       <c r="AA9" s="23"/>
       <c r="AB9" s="23"/>
@@ -24338,23 +24388,23 @@
       <c r="AJ9" s="23"/>
       <c r="AK9" s="19"/>
       <c r="AL9" s="19"/>
-      <c r="AM9" s="1"/>
-      <c r="AN9" s="1"/>
-      <c r="AO9" s="1"/>
-      <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
+      <c r="AM9" s="148"/>
+      <c r="AN9" s="148"/>
+      <c r="AO9" s="148"/>
+      <c r="AP9" s="148"/>
+      <c r="AQ9" s="148"/>
       <c r="AR9" s="21"/>
       <c r="AS9" s="22"/>
-      <c r="AT9" s="1"/>
-      <c r="AU9" s="1"/>
-      <c r="AV9" s="1"/>
-      <c r="AW9" s="1"/>
-      <c r="AX9" s="1"/>
-      <c r="AY9" s="1"/>
-      <c r="AZ9" s="1"/>
-      <c r="BA9" s="1"/>
-      <c r="BB9" s="1"/>
-      <c r="BC9" s="1"/>
+      <c r="AT9" s="148"/>
+      <c r="AU9" s="148"/>
+      <c r="AV9" s="148"/>
+      <c r="AW9" s="148"/>
+      <c r="AX9" s="148"/>
+      <c r="AY9" s="148"/>
+      <c r="AZ9" s="148"/>
+      <c r="BA9" s="148"/>
+      <c r="BB9" s="148"/>
+      <c r="BC9" s="148"/>
     </row>
     <row r="10" spans="1:55" ht="13.5" customHeight="1">
       <c r="A10" s="1"/>
@@ -25927,7 +25977,7 @@
       </c>
       <c r="G36" s="36">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>5.75</v>
       </c>
       <c r="H36" s="37">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -25999,7 +26049,7 @@
       </c>
       <c r="Y36" s="72">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z36" s="72">
         <f t="shared" si="3"/>
@@ -26488,12 +26538,22 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26507,23 +26567,23 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
+  <conditionalFormatting sqref="G6">
     <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
+  <conditionalFormatting sqref="G6">
     <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29247,12 +29307,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32025,12 +32085,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34802,12 +34862,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37531,12 +37591,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Memoria final.docx Hoja de esfuerzo
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Christian.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="53">
   <si>
     <t>GP</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>Reunion repartir tareas memoria</t>
+  </si>
+  <si>
+    <t>Estructura de la memoria y breve descripcion de todos los puntos</t>
   </si>
 </sst>
 </file>
@@ -2298,7 +2301,7 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2385,11 +2388,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82309888"/>
-        <c:axId val="82312192"/>
+        <c:axId val="47510272"/>
+        <c:axId val="47512576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82309888"/>
+        <c:axId val="47510272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2426,13 +2429,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82312192"/>
+        <c:crossAx val="47512576"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82312192"/>
+        <c:axId val="47512576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2484,7 +2487,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82309888"/>
+        <c:crossAx val="47510272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2506,7 +2509,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14749,7 +14752,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -14769,7 +14772,7 @@
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="M6" s="116">
         <f>Jun!G36</f>
@@ -23697,7 +23700,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24554,14 +24557,24 @@
     </row>
     <row r="12" spans="1:55" ht="13.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
+      <c r="B12" s="21">
+        <v>84</v>
+      </c>
+      <c r="C12" s="23">
+        <v>2</v>
+      </c>
+      <c r="D12" s="23">
+        <v>57</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="G12" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
@@ -24588,7 +24601,9 @@
       <c r="AD12" s="19"/>
       <c r="AE12" s="19"/>
       <c r="AF12" s="23"/>
-      <c r="AG12" s="23"/>
+      <c r="AG12" s="23">
+        <v>1</v>
+      </c>
       <c r="AH12" s="23"/>
       <c r="AI12" s="23"/>
       <c r="AJ12" s="23"/>
@@ -26003,7 +26018,7 @@
       </c>
       <c r="G36" s="36">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="H36" s="37">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -26107,7 +26122,7 @@
       </c>
       <c r="AG36" s="72">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH36" s="72">
         <f t="shared" si="3"/>

</xml_diff>